<commit_message>
perf: obtaining the final string using only 2 loops and not 4
</commit_message>
<xml_diff>
--- a/weekly-activities.xlsx
+++ b/weekly-activities.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Atividade 1</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Curso React - 4 horas</t>
   </si>
   <si>
-    <t>Reuniao - 1 hora</t>
-  </si>
-  <si>
     <t>Terca</t>
   </si>
   <si>
@@ -76,7 +73,7 @@
     <t>Sprint planing - 2 horas</t>
   </si>
   <si>
-    <t>Reunião Sinavez - 1 hora</t>
+    <t>Reuniao Sinavez - 1 hora</t>
   </si>
   <si>
     <t>Implementar front - 1 hora</t>
@@ -368,64 +365,62 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: the automation function has been successfully integrated.
</commit_message>
<xml_diff>
--- a/weekly-activities.xlsx
+++ b/weekly-activities.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Atividade 1</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Terca</t>
   </si>
   <si>
-    <t>Aguia - 1 hora</t>
+    <t>Rever front - 1 hora</t>
   </si>
   <si>
     <t>Curso Web - 3 horas</t>
@@ -49,9 +49,6 @@
     <t>Sprint review - 1 hora</t>
   </si>
   <si>
-    <t>Elaborar Contrato - 1 hora</t>
-  </si>
-  <si>
     <t>Marcar reuniao - 1 hora</t>
   </si>
   <si>
@@ -71,12 +68,6 @@
   </si>
   <si>
     <t>Sprint planing - 2 horas</t>
-  </si>
-  <si>
-    <t>Reuniao Sinavez - 1 hora</t>
-  </si>
-  <si>
-    <t>Implementar front - 1 hora</t>
   </si>
 </sst>
 </file>
@@ -391,36 +382,27 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>